<commit_message>
delete extra blank space
</commit_message>
<xml_diff>
--- a/BackEnd/public/test1.xlsx
+++ b/BackEnd/public/test1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PythonProject\parse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GithubProjects\tablevis\BackEnd\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85ECFCF5-0879-475A-9585-5B5EDE96EBC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E2F557-1C0D-424F-A649-9CF620B19189}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{018033FE-E987-497D-8A4E-724D96333FBD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{018033FE-E987-497D-8A4E-724D96333FBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="30">
-  <si>
-    <t xml:space="preserve">    SSH </t>
-  </si>
-  <si>
-    <t xml:space="preserve">%Chg </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="31">
   <si>
     <t>FTE</t>
   </si>
@@ -42,86 +36,10 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">   American Studies</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">   English </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">   Hawn-Pac Studies </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">   History </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">   Humanities</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">   Literature </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">   Philosophy</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">   Business Admin </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">   Profess Studies </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">   Public Admin</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">   Anthropology </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">   Economics</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">   Political Science </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">   Psychology </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">   Social Science</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">   Sociology</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>TOTAL</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">      HUMANITIES </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">      PROFESS STUDIES </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">      SOCIAL SCIENCES </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>FALL 2001</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -139,6 +57,94 @@
   </si>
   <si>
     <t>FALL 2005</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FTE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SSH</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>%Chg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>HUMANITIES</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PROFESS STUDIES</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOCIAL SCIENCES</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>American Studies</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Philosophy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Humanities</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Public Admin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Economics</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Social Science</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sociology</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>English</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hawn-Pac Studies</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>History</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Literature</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Business Admin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Profess Studies</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anthropology</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Political Science</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Psychology</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -375,6 +381,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -389,42 +431,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -743,97 +749,97 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="40.375" customWidth="1"/>
+    <col min="2" max="2" width="20.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15">
-      <c r="A1" s="20"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" s="12"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M1" s="12"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="14"/>
+      <c r="A1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="24"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="24"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="24"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="24"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="26"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="3" spans="1:17" ht="15">
-      <c r="A3" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="27"/>
+      <c r="A3" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="18"/>
       <c r="C3" s="3">
         <v>6647</v>
       </c>
@@ -881,10 +887,10 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="15">
-      <c r="A4" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="25"/>
+      <c r="A4" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="16"/>
       <c r="C4" s="3">
         <v>1083</v>
       </c>
@@ -932,117 +938,117 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="15">
-      <c r="A5" s="18"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="9" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15">
-      <c r="A6" s="18"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="9" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15">
-      <c r="A7" s="18"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="9" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C7" s="3">
         <v>21</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E7" s="5">
         <v>1</v>
@@ -1085,9 +1091,9 @@
       </c>
     </row>
     <row r="8" spans="1:17" ht="15">
-      <c r="A8" s="18"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="9" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C8" s="3">
         <v>177</v>
@@ -1136,9 +1142,9 @@
       </c>
     </row>
     <row r="9" spans="1:17" ht="15">
-      <c r="A9" s="18"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="9" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C9" s="3">
         <v>504</v>
@@ -1187,9 +1193,9 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="15">
-      <c r="A10" s="18"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="9" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C10" s="3">
         <v>206</v>
@@ -1238,9 +1244,9 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="15">
-      <c r="A11" s="18"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="9" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C11" s="3">
         <v>175</v>
@@ -1289,10 +1295,10 @@
       </c>
     </row>
     <row r="12" spans="1:17" ht="15">
-      <c r="A12" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="17"/>
+      <c r="A12" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="22"/>
       <c r="C12" s="3">
         <v>2113</v>
       </c>
@@ -1340,9 +1346,9 @@
       </c>
     </row>
     <row r="13" spans="1:17" ht="15">
-      <c r="A13" s="18"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="9" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C13" s="3">
         <v>1117</v>
@@ -1391,15 +1397,15 @@
       </c>
     </row>
     <row r="14" spans="1:17" ht="15">
-      <c r="A14" s="18"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="9" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C14" s="3">
         <v>0</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E14" s="5">
         <v>0</v>
@@ -1408,7 +1414,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H14" s="5">
         <v>0</v>
@@ -1417,7 +1423,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K14" s="5">
         <v>0</v>
@@ -1426,7 +1432,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N14" s="5">
         <v>0</v>
@@ -1435,16 +1441,16 @@
         <v>0</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q14" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="15">
-      <c r="A15" s="18"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="9" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C15" s="3">
         <v>996</v>
@@ -1493,10 +1499,10 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="15">
-      <c r="A16" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="17"/>
+      <c r="A16" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="22"/>
       <c r="C16" s="3">
         <v>3426</v>
       </c>
@@ -1544,9 +1550,9 @@
       </c>
     </row>
     <row r="17" spans="1:17" ht="15">
-      <c r="A17" s="18"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="9" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C17" s="3">
         <v>495</v>
@@ -1595,9 +1601,9 @@
       </c>
     </row>
     <row r="18" spans="1:17" ht="15">
-      <c r="A18" s="18"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C18" s="3">
         <v>235</v>
@@ -1646,9 +1652,9 @@
       </c>
     </row>
     <row r="19" spans="1:17" ht="15">
-      <c r="A19" s="18"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="9" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C19" s="3">
         <v>205</v>
@@ -1697,9 +1703,9 @@
       </c>
     </row>
     <row r="20" spans="1:17" ht="15">
-      <c r="A20" s="18"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="9" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C20" s="3">
         <v>1347</v>
@@ -1748,9 +1754,9 @@
       </c>
     </row>
     <row r="21" spans="1:17" ht="15">
-      <c r="A21" s="18"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C21" s="3">
         <v>492</v>
@@ -1799,9 +1805,9 @@
       </c>
     </row>
     <row r="22" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A22" s="19"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C22" s="6">
         <v>652</v>
@@ -1851,16 +1857,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="C1:E1"/>
     <mergeCell ref="A17:A22"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A5:A11"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="C1:E1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>